<commit_message>
forecast data dictionary and location ids
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
@@ -5,14 +5,20 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\gbd2017_models\causes\neoplasms\breast_cancer_with_stage0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\gbd2017_models\concept_models\vivarium_swissre_breastcancer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="19155" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="2370" windowHeight="0" tabRatio="825" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="filepaths" sheetId="1" r:id="rId1"/>
+    <sheet name="acmr_294" sheetId="3" r:id="rId2"/>
+    <sheet name="csmr_c429" sheetId="6" r:id="rId3"/>
+    <sheet name="incidence_c429" sheetId="7" r:id="rId4"/>
+    <sheet name="prevalence_c429" sheetId="2" r:id="rId5"/>
+    <sheet name="age_groups" sheetId="4" r:id="rId6"/>
+    <sheet name="location_id" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
   <si>
     <t>forcasted 2020-2040</t>
   </si>
@@ -62,9 +68,6 @@
     <t>/ihme/costeffectiveness/vivarium_csu_cancer/294_ets_mortality_beta_8_phi_89.nc</t>
   </si>
   <si>
-    <t>per 100,000 pyrs</t>
-  </si>
-  <si>
     <t>Granularity</t>
   </si>
   <si>
@@ -75,13 +78,169 @@
   </si>
   <si>
     <t>percent</t>
+  </si>
+  <si>
+    <t>age_group</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>data item</t>
+  </si>
+  <si>
+    <t>data type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>age group id</t>
+  </si>
+  <si>
+    <t>age_group_id</t>
+  </si>
+  <si>
+    <t>age_group_name</t>
+  </si>
+  <si>
+    <t>age_start</t>
+  </si>
+  <si>
+    <t>age_end</t>
+  </si>
+  <si>
+    <t>15 to 19</t>
+  </si>
+  <si>
+    <t>20 to 24</t>
+  </si>
+  <si>
+    <t>25 to 29</t>
+  </si>
+  <si>
+    <t>30 to 34</t>
+  </si>
+  <si>
+    <t>35 to 39</t>
+  </si>
+  <si>
+    <t>40 to 44</t>
+  </si>
+  <si>
+    <t>45 to 49</t>
+  </si>
+  <si>
+    <t>50 to 54</t>
+  </si>
+  <si>
+    <t>55 to 59</t>
+  </si>
+  <si>
+    <t>60 to 64</t>
+  </si>
+  <si>
+    <t>65 to 69</t>
+  </si>
+  <si>
+    <t>70 to 74</t>
+  </si>
+  <si>
+    <t>75 to 79</t>
+  </si>
+  <si>
+    <t>80 to 84</t>
+  </si>
+  <si>
+    <t>85 to 89</t>
+  </si>
+  <si>
+    <t>90 to 94</t>
+  </si>
+  <si>
+    <t>95 plus</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>location id</t>
+  </si>
+  <si>
+    <t>year_id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>see age group tab</t>
+  </si>
+  <si>
+    <t>1990-2040</t>
+  </si>
+  <si>
+    <t>see location tab</t>
+  </si>
+  <si>
+    <t>sex_id</t>
+  </si>
+  <si>
+    <t>sex id</t>
+  </si>
+  <si>
+    <t>1=male; 2=female</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>draw number</t>
+  </si>
+  <si>
+    <t>0-999</t>
+  </si>
+  <si>
+    <t>dimension(size)</t>
+  </si>
+  <si>
+    <t>prevalence</t>
+  </si>
+  <si>
+    <t>incidence</t>
+  </si>
+  <si>
+    <t>float, log space</t>
+  </si>
+  <si>
+    <t>per person year</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>after log transformation: all-cause mortality rate as death per person-years stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>after log transformation: cause specific mortality rate as death per person year stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>after log transformation: incidence rate per person year stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>after log transformation: percentage stratified by age, sex, location year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,16 +256,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -114,13 +310,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,15 +659,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -424,10 +680,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -441,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -455,10 +711,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -469,10 +725,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -483,13 +739,1152 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12">
+        <v>23</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12">
+        <v>33</v>
+      </c>
+      <c r="F5" s="12">
+        <v>33</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="18">
+        <f>PRODUCT(E3:E7)</f>
+        <v>57222000</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F13:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12">
+        <v>33</v>
+      </c>
+      <c r="F5" s="12">
+        <v>33</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="18">
+        <f>PRODUCT(E3:E7)</f>
+        <v>57222000</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F13:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12">
+        <v>33</v>
+      </c>
+      <c r="F5" s="12">
+        <v>33</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="18">
+        <f>PRODUCT(E3:E7)</f>
+        <v>57222000</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12">
+        <v>33</v>
+      </c>
+      <c r="F5" s="12">
+        <v>33</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="18">
+        <f>PRODUCT(E3:E7)</f>
+        <v>57222000</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F19"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="7">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="6">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="7">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="7">
+        <v>40</v>
+      </c>
+      <c r="E8" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7">
+        <v>15</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7">
+        <v>17</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="7">
+        <v>60</v>
+      </c>
+      <c r="E12" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6">
+        <v>65</v>
+      </c>
+      <c r="E13" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="7">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="7">
+        <v>70</v>
+      </c>
+      <c r="E14" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6">
+        <v>20</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="6">
+        <v>75</v>
+      </c>
+      <c r="E15" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="7">
+        <v>30</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7">
+        <v>80</v>
+      </c>
+      <c r="E16" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6">
+        <v>85</v>
+      </c>
+      <c r="E17" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="7">
+        <v>32</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="7">
+        <v>90</v>
+      </c>
+      <c r="E18" s="7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7">
+        <v>235</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="7">
+        <v>95</v>
+      </c>
+      <c r="E19" s="7">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="9">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>361</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="10">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="10">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="10">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="10">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="10">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="10">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="9">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="10">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="9">
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added equations to get popuation weighted acmr
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="2370" windowHeight="0" tabRatio="825" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="2370" windowHeight="0" tabRatio="825" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="101">
   <si>
     <t>forcasted 2020-2040</t>
   </si>
@@ -234,6 +234,105 @@
   </si>
   <si>
     <t>after log transformation: percentage stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>Anhui</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Chongqing</t>
+  </si>
+  <si>
+    <t>Fujian</t>
+  </si>
+  <si>
+    <t>Gansu</t>
+  </si>
+  <si>
+    <t>Guangdong</t>
+  </si>
+  <si>
+    <t>Guangxi</t>
+  </si>
+  <si>
+    <t>Guizhou</t>
+  </si>
+  <si>
+    <t>Hainan</t>
+  </si>
+  <si>
+    <t>Hebei</t>
+  </si>
+  <si>
+    <t>Heilongjiang</t>
+  </si>
+  <si>
+    <t>Henan</t>
+  </si>
+  <si>
+    <t>Hubei</t>
+  </si>
+  <si>
+    <t>Hunan</t>
+  </si>
+  <si>
+    <t>Jiangsu</t>
+  </si>
+  <si>
+    <t>Jiangxi</t>
+  </si>
+  <si>
+    <t>Jilin</t>
+  </si>
+  <si>
+    <t>Liaoning</t>
+  </si>
+  <si>
+    <t>Ningxia</t>
+  </si>
+  <si>
+    <t>Qinghai</t>
+  </si>
+  <si>
+    <t>Shaanxi</t>
+  </si>
+  <si>
+    <t>Shandong</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Shanxi</t>
+  </si>
+  <si>
+    <t>Sichuan</t>
+  </si>
+  <si>
+    <t>Tianjin</t>
+  </si>
+  <si>
+    <t>Tibet</t>
+  </si>
+  <si>
+    <t>Xinjiang</t>
+  </si>
+  <si>
+    <t>Yunnan</t>
+  </si>
+  <si>
+    <t>Zhejiang</t>
+  </si>
+  <si>
+    <t>Inner Mongolia</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1408,7 +1507,7 @@
   <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,192 +1798,292 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N35"/>
+  <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="9">
         <v>354</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <v>361</v>
       </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>491</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>492</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>493</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>494</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>495</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>496</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>497</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>498</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>499</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>500</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>501</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>502</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>503</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>504</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>505</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>506</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>507</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>508</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>509</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>510</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>511</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>512</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>513</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>514</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>515</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>516</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>517</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>518</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>519</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>520</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <v>521</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised acmr equation description; changed deaths to csmr in filepaths data dictionary
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/filepaths_c429_forecast.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="2370" windowHeight="0" tabRatio="825" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="2370" windowHeight="0" tabRatio="849" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="102">
   <si>
     <t>forcasted 2020-2040</t>
   </si>
@@ -47,9 +47,6 @@
     <t>filepath</t>
   </si>
   <si>
-    <t>deaths c429</t>
-  </si>
-  <si>
     <t>incidence c429</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>to be determined</t>
   </si>
   <si>
-    <t>acmr</t>
-  </si>
-  <si>
     <t>/ihme/costeffectiveness/vivarium_csu_cancer/294_ets_mortality_beta_8_phi_89.nc</t>
   </si>
   <si>
@@ -218,24 +212,9 @@
     <t>float, log space</t>
   </si>
   <si>
-    <t>per person year</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>after log transformation: all-cause mortality rate as death per person-years stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>after log transformation: cause specific mortality rate as death per person year stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>after log transformation: incidence rate per person year stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>after log transformation: percentage stratified by age, sex, location year</t>
-  </si>
-  <si>
     <t>Macao</t>
   </si>
   <si>
@@ -333,6 +312,30 @@
   </si>
   <si>
     <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>csmr c429</t>
+  </si>
+  <si>
+    <t>rate, per person year</t>
+  </si>
+  <si>
+    <t>rate per person year</t>
+  </si>
+  <si>
+    <t>acmr 294</t>
+  </si>
+  <si>
+    <t>after exp transformation: percentage stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>This is the log(acmr). After exp transformation: all-cause mortality rate as death per person-years stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>This is the log(csmr). After exp transformation: cause specific mortality rate as death per person year stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>This is the log(incidence rate). After exp transformation: incidence rate per person year stratified by age, sex, location year</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -475,6 +478,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,14 +769,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -779,10 +789,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -796,55 +806,55 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +868,7 @@
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,33 +884,33 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="12">
         <v>17</v>
@@ -909,19 +919,19 @@
         <v>23</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -930,18 +940,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="12">
         <v>33</v>
@@ -950,19 +960,19 @@
         <v>33</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="12">
         <v>51</v>
@@ -971,19 +981,19 @@
         <v>51</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="13">
         <v>1000</v>
@@ -992,18 +1002,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="E8" s="18">
         <f>PRODUCT(E3:E7)</f>
@@ -1023,7 +1033,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F13:F14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1041,7 @@
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -1039,33 +1049,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="12">
         <v>17</v>
@@ -1074,18 +1084,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -1094,18 +1104,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="12">
         <v>33</v>
@@ -1114,18 +1124,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="12">
         <v>51</v>
@@ -1134,18 +1144,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="13">
         <v>1000</v>
@@ -1154,18 +1164,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="E8" s="18">
         <f>PRODUCT(E3:E7)</f>
@@ -1183,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F13:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H13:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1202,7 @@
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -1200,33 +1210,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="12">
         <v>17</v>
@@ -1235,18 +1245,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -1255,18 +1265,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="12">
         <v>33</v>
@@ -1275,18 +1285,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="12">
         <v>51</v>
@@ -1295,18 +1305,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="13">
         <v>1000</v>
@@ -1315,18 +1325,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="E8" s="18">
         <f>PRODUCT(E3:E7)</f>
@@ -1345,7 +1355,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,33 +1371,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="12">
         <v>17</v>
@@ -1396,18 +1406,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -1416,18 +1426,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="12">
         <v>33</v>
@@ -1436,18 +1446,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="12">
         <v>51</v>
@@ -1456,18 +1466,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="13">
         <v>1000</v>
@@ -1476,18 +1486,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>61</v>
-      </c>
       <c r="D8" s="16" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E8" s="18">
         <f>PRODUCT(E3:E7)</f>
@@ -1507,7 +1517,7 @@
   <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,16 +1530,16 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -1539,7 +1549,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="6">
         <v>15</v>
@@ -1555,7 +1565,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7">
         <v>20</v>
@@ -1571,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="6">
         <v>25</v>
@@ -1586,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7">
         <v>30</v>
@@ -1601,7 +1611,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6">
         <v>35</v>
@@ -1616,7 +1626,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="7">
         <v>40</v>
@@ -1631,7 +1641,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6">
         <v>45</v>
@@ -1646,7 +1656,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="7">
         <v>50</v>
@@ -1661,7 +1671,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6">
         <v>55</v>
@@ -1676,7 +1686,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="7">
         <v>60</v>
@@ -1691,7 +1701,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6">
         <v>65</v>
@@ -1706,7 +1716,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7">
         <v>70</v>
@@ -1721,7 +1731,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="6">
         <v>75</v>
@@ -1736,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="7">
         <v>80</v>
@@ -1751,7 +1761,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="6">
         <v>85</v>
@@ -1766,7 +1776,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="7">
         <v>90</v>
@@ -1781,7 +1791,7 @@
         <v>235</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="7">
         <v>95</v>
@@ -1800,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,23 +1823,24 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="9">
         <v>354</v>
       </c>
-      <c r="C3" t="s">
-        <v>100</v>
+      <c r="C3" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <v>361</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
+      <c r="C4" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1842,248 +1853,248 @@
       <c r="B5" s="10">
         <v>491</v>
       </c>
-      <c r="C5" t="s">
-        <v>69</v>
+      <c r="C5" s="17" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>492</v>
       </c>
-      <c r="C6" t="s">
-        <v>70</v>
+      <c r="C6" s="17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>493</v>
       </c>
-      <c r="C7" t="s">
-        <v>71</v>
+      <c r="C7" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>494</v>
       </c>
-      <c r="C8" t="s">
-        <v>72</v>
+      <c r="C8" s="17" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>495</v>
       </c>
-      <c r="C9" t="s">
-        <v>73</v>
+      <c r="C9" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="B10" s="19">
         <v>496</v>
       </c>
-      <c r="C10" t="s">
-        <v>74</v>
+      <c r="C10" s="20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>497</v>
       </c>
-      <c r="C11" t="s">
-        <v>75</v>
+      <c r="C11" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>498</v>
       </c>
-      <c r="C12" t="s">
-        <v>76</v>
+      <c r="C12" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>499</v>
       </c>
-      <c r="C13" t="s">
-        <v>77</v>
+      <c r="C13" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>500</v>
       </c>
-      <c r="C14" t="s">
-        <v>78</v>
+      <c r="C14" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="10">
+      <c r="B15" s="19">
         <v>501</v>
       </c>
-      <c r="C15" t="s">
-        <v>79</v>
+      <c r="C15" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
+      <c r="B16" s="21">
         <v>502</v>
       </c>
-      <c r="C16" t="s">
-        <v>80</v>
+      <c r="C16" s="20" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>503</v>
       </c>
-      <c r="C17" t="s">
-        <v>81</v>
+      <c r="C17" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>504</v>
       </c>
-      <c r="C18" t="s">
-        <v>82</v>
+      <c r="C18" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>505</v>
       </c>
-      <c r="C19" t="s">
-        <v>99</v>
+      <c r="C19" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="10">
+      <c r="B20" s="19">
         <v>506</v>
       </c>
-      <c r="C20" t="s">
-        <v>83</v>
+      <c r="C20" s="20" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>507</v>
       </c>
-      <c r="C21" t="s">
-        <v>84</v>
+      <c r="C21" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>508</v>
       </c>
-      <c r="C22" t="s">
-        <v>85</v>
+      <c r="C22" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>509</v>
       </c>
-      <c r="C23" t="s">
-        <v>86</v>
+      <c r="C23" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>510</v>
       </c>
-      <c r="C24" t="s">
-        <v>87</v>
+      <c r="C24" s="17" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>511</v>
       </c>
-      <c r="C25" t="s">
-        <v>88</v>
+      <c r="C25" s="17" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>512</v>
       </c>
-      <c r="C26" t="s">
-        <v>89</v>
+      <c r="C26" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>513</v>
       </c>
-      <c r="C27" t="s">
-        <v>90</v>
+      <c r="C27" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>514</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
+      <c r="C28" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>515</v>
       </c>
-      <c r="C29" t="s">
-        <v>92</v>
+      <c r="C29" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>516</v>
       </c>
-      <c r="C30" t="s">
-        <v>93</v>
+      <c r="C30" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="10">
+      <c r="B31" s="19">
         <v>517</v>
       </c>
-      <c r="C31" t="s">
-        <v>94</v>
+      <c r="C31" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>518</v>
       </c>
-      <c r="C32" t="s">
-        <v>95</v>
+      <c r="C32" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>519</v>
       </c>
-      <c r="C33" t="s">
-        <v>96</v>
+      <c r="C33" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>520</v>
       </c>
-      <c r="C34" t="s">
-        <v>97</v>
+      <c r="C34" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <v>521</v>
       </c>
-      <c r="C35" t="s">
-        <v>98</v>
+      <c r="C35" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>